<commit_message>
Atualização do projeto no Orange e geração de alguns relatórios no Orange.
</commit_message>
<xml_diff>
--- a/Orange/leaf.xlsx
+++ b/Orange/leaf.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manoel\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdefreitasgo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9F406C59-FFCA-42AE-8916-23F53083AAB3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="leaf" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="31">
   <si>
     <t>Classe</t>
   </si>
@@ -102,9 +103,6 @@
     <t>Pseudosasa japonica</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>d</t>
   </si>
   <si>
@@ -120,7 +118,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -632,10 +630,10 @@
     <cellStyle name="Ênfase5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Ênfase6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorreto" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutra" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Neutro" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Ruim" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Saída" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Texto de Aviso" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Texto Explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -921,11 +919,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,52 +1006,52 @@
         <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -1061,7 +1059,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -7055,6 +7053,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>